<commit_message>
added functionality in virustotal to check if website is redirecting by statuscode 301 or 302
</commit_message>
<xml_diff>
--- a/out/mycom/shodan_data.xlsx
+++ b/out/mycom/shodan_data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2023\cyberkit\out\mycom\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAAC71A-E0FD-41D3-A314-EA84080522D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -127,7 +121,7 @@
     <t>['forpsi.net']</t>
   </si>
   <si>
-    <t>['drgros.de', 'googleusercontent.com']</t>
+    <t>['stm360.co.uk', 'googleusercontent.com']</t>
   </si>
   <si>
     <t>Windows</t>
@@ -163,8 +157,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,14 +221,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -281,7 +267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -313,27 +299,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,24 +333,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -558,28 +508,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" customWidth="1"/>
-    <col min="9" max="9" width="35" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -637,7 +573,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -669,7 +605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -701,7 +637,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -733,7 +669,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -765,7 +701,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -797,7 +733,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -823,7 +759,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -855,7 +791,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -887,7 +823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -919,7 +855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -945,7 +881,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -977,7 +913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +939,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>20</v>
       </c>

</xml_diff>